<commit_message>
Added GTIN Document Started EER diagram
Signed-off-by: Rlisbona <rlisbona@smu.edu>
</commit_message>
<xml_diff>
--- a/DataSources/POD-SPECS-2013.11.13_01.xlsx
+++ b/DataSources/POD-SPECS-2013.11.13_01.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="540" windowWidth="15600" windowHeight="9000" tabRatio="697"/>
+    <workbookView xWindow="480" yWindow="540" windowWidth="15600" windowHeight="9000" tabRatio="697" firstSheet="10" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="ChangeLog" sheetId="1" r:id="rId1"/>
@@ -1593,6 +1593,15 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1605,22 +1614,41 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -3921,7 +3949,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -4212,16 +4240,16 @@
   </sheetPr>
   <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.5703125" style="4" customWidth="1"/>
-    <col min="2" max="2" width="12.5703125" style="4" customWidth="1"/>
-    <col min="3" max="3" width="117.7109375" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="11.42578125" style="1"/>
+    <col min="1" max="1" width="16.625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="12.625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="117.75" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="11.375" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="39" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -4370,27 +4398,27 @@
       <selection pane="bottomLeft" activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="1.5703125" style="30" customWidth="1"/>
+    <col min="1" max="1" width="1.625" style="30" customWidth="1"/>
     <col min="2" max="2" width="25" style="10" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" style="10" customWidth="1"/>
-    <col min="4" max="4" width="8.42578125" style="10" customWidth="1"/>
-    <col min="5" max="5" width="41.85546875" style="10" customWidth="1"/>
-    <col min="6" max="6" width="103.42578125" style="10" customWidth="1"/>
-    <col min="7" max="7" width="32.5703125" style="10" customWidth="1"/>
-    <col min="8" max="16384" width="11.42578125" style="10"/>
+    <col min="3" max="3" width="15.75" style="10" customWidth="1"/>
+    <col min="4" max="4" width="8.375" style="10" customWidth="1"/>
+    <col min="5" max="5" width="41.875" style="10" customWidth="1"/>
+    <col min="6" max="6" width="103.375" style="10" customWidth="1"/>
+    <col min="7" max="7" width="32.625" style="10" customWidth="1"/>
+    <col min="8" max="16384" width="11.375" style="10"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="24" customFormat="1" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="25"/>
-      <c r="B1" s="48" t="s">
+      <c r="B1" s="51" t="s">
         <v>229</v>
       </c>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
-      <c r="F1" s="48"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
+      <c r="F1" s="51"/>
     </row>
     <row r="2" spans="1:7" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="26"/>
@@ -4434,19 +4462,19 @@
         <v>227</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="54" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="27"/>
-      <c r="B4" s="52" t="s">
+      <c r="B4" s="48" t="s">
         <v>343</v>
       </c>
-      <c r="C4" s="52" t="s">
+      <c r="C4" s="48" t="s">
         <v>344</v>
       </c>
-      <c r="D4" s="52"/>
-      <c r="E4" s="53" t="s">
+      <c r="D4" s="48"/>
+      <c r="E4" s="49" t="s">
         <v>345</v>
       </c>
-      <c r="F4" s="52"/>
+      <c r="F4" s="48"/>
       <c r="G4" s="9" t="s">
         <v>227</v>
       </c>
@@ -4543,32 +4571,32 @@
   </sheetPr>
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E8" sqref="E8"/>
+      <selection pane="bottomLeft" activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="1.5703125" style="30" customWidth="1"/>
+    <col min="1" max="1" width="1.625" style="30" customWidth="1"/>
     <col min="2" max="2" width="25" style="10" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" style="10" customWidth="1"/>
-    <col min="4" max="4" width="8.42578125" style="10" customWidth="1"/>
-    <col min="5" max="5" width="41.85546875" style="10" customWidth="1"/>
-    <col min="6" max="6" width="103.42578125" style="10" customWidth="1"/>
-    <col min="7" max="7" width="32.5703125" style="10" customWidth="1"/>
-    <col min="8" max="16384" width="11.42578125" style="10"/>
+    <col min="3" max="3" width="15.75" style="10" customWidth="1"/>
+    <col min="4" max="4" width="8.375" style="10" customWidth="1"/>
+    <col min="5" max="5" width="41.875" style="10" customWidth="1"/>
+    <col min="6" max="6" width="103.375" style="10" customWidth="1"/>
+    <col min="7" max="7" width="32.625" style="10" customWidth="1"/>
+    <col min="8" max="16384" width="11.375" style="10"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="24" customFormat="1" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="25"/>
-      <c r="B1" s="48" t="s">
+      <c r="B1" s="51" t="s">
         <v>336</v>
       </c>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
-      <c r="F1" s="48"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
+      <c r="F1" s="51"/>
     </row>
     <row r="2" spans="1:7" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="26"/>
@@ -4688,27 +4716,27 @@
       <selection pane="bottomLeft" activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="1.5703125" style="30" customWidth="1"/>
+    <col min="1" max="1" width="1.625" style="30" customWidth="1"/>
     <col min="2" max="2" width="25" style="10" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" style="10" customWidth="1"/>
-    <col min="4" max="4" width="8.42578125" style="10" customWidth="1"/>
-    <col min="5" max="5" width="34.42578125" style="10" customWidth="1"/>
-    <col min="6" max="6" width="49.140625" style="10" customWidth="1"/>
-    <col min="7" max="7" width="27.7109375" style="10" customWidth="1"/>
-    <col min="8" max="16384" width="11.42578125" style="10"/>
+    <col min="3" max="3" width="15.75" style="10" customWidth="1"/>
+    <col min="4" max="4" width="8.375" style="10" customWidth="1"/>
+    <col min="5" max="5" width="34.375" style="10" customWidth="1"/>
+    <col min="6" max="6" width="49.125" style="10" customWidth="1"/>
+    <col min="7" max="7" width="27.75" style="10" customWidth="1"/>
+    <col min="8" max="16384" width="11.375" style="10"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="24" customFormat="1" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="25"/>
-      <c r="B1" s="48" t="s">
+      <c r="B1" s="51" t="s">
         <v>230</v>
       </c>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
-      <c r="F1" s="48"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
+      <c r="F1" s="51"/>
     </row>
     <row r="2" spans="1:7" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="26"/>
@@ -4790,27 +4818,27 @@
       <selection pane="bottomLeft" activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="1.5703125" style="30" customWidth="1"/>
+    <col min="1" max="1" width="1.625" style="30" customWidth="1"/>
     <col min="2" max="2" width="25" style="10" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" style="10" customWidth="1"/>
-    <col min="4" max="4" width="8.42578125" style="10" customWidth="1"/>
-    <col min="5" max="5" width="41.85546875" style="10" customWidth="1"/>
-    <col min="6" max="6" width="57.28515625" style="10" customWidth="1"/>
-    <col min="7" max="7" width="15.7109375" style="10" customWidth="1"/>
-    <col min="8" max="16384" width="11.42578125" style="10"/>
+    <col min="3" max="3" width="15.75" style="10" customWidth="1"/>
+    <col min="4" max="4" width="8.375" style="10" customWidth="1"/>
+    <col min="5" max="5" width="41.875" style="10" customWidth="1"/>
+    <col min="6" max="6" width="57.25" style="10" customWidth="1"/>
+    <col min="7" max="7" width="15.75" style="10" customWidth="1"/>
+    <col min="8" max="16384" width="11.375" style="10"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="24" customFormat="1" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="25"/>
-      <c r="B1" s="49" t="s">
+      <c r="B1" s="52" t="s">
         <v>234</v>
       </c>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
-      <c r="F1" s="49"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
+      <c r="F1" s="52"/>
     </row>
     <row r="2" spans="1:6" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="26"/>
@@ -4869,13 +4897,13 @@
       <c r="F5" s="9"/>
     </row>
     <row r="7" spans="1:6" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="51" t="s">
+      <c r="B7" s="54" t="s">
         <v>251</v>
       </c>
-      <c r="C7" s="51"/>
-      <c r="D7" s="51"/>
-      <c r="E7" s="51"/>
-      <c r="F7" s="51"/>
+      <c r="C7" s="54"/>
+      <c r="D7" s="54"/>
+      <c r="E7" s="54"/>
+      <c r="F7" s="54"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -4899,27 +4927,27 @@
       <selection pane="bottomLeft" activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="1.5703125" style="30" customWidth="1"/>
+    <col min="1" max="1" width="1.625" style="30" customWidth="1"/>
     <col min="2" max="2" width="25" style="10" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" style="10" customWidth="1"/>
-    <col min="4" max="4" width="8.42578125" style="10" customWidth="1"/>
-    <col min="5" max="5" width="41.85546875" style="10" customWidth="1"/>
-    <col min="6" max="6" width="57.28515625" style="10" customWidth="1"/>
-    <col min="7" max="7" width="15.7109375" style="10" customWidth="1"/>
-    <col min="8" max="16384" width="11.42578125" style="10"/>
+    <col min="3" max="3" width="15.75" style="10" customWidth="1"/>
+    <col min="4" max="4" width="8.375" style="10" customWidth="1"/>
+    <col min="5" max="5" width="41.875" style="10" customWidth="1"/>
+    <col min="6" max="6" width="57.25" style="10" customWidth="1"/>
+    <col min="7" max="7" width="15.75" style="10" customWidth="1"/>
+    <col min="8" max="16384" width="11.375" style="10"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="24" customFormat="1" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="25"/>
-      <c r="B1" s="49" t="s">
+      <c r="B1" s="52" t="s">
         <v>268</v>
       </c>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
-      <c r="F1" s="49"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
+      <c r="F1" s="52"/>
     </row>
     <row r="2" spans="1:6" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="26"/>
@@ -5333,15 +5361,15 @@
       <selection activeCell="R35" sqref="R35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="8" max="8" width="10" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="48.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.140625" customWidth="1"/>
-    <col min="19" max="19" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="10.125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="48.375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.125" customWidth="1"/>
+    <col min="19" max="19" width="9.875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="13.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="33" customFormat="1" x14ac:dyDescent="0.25">
@@ -7281,14 +7309,14 @@
   </sheetPr>
   <dimension ref="A1:B24"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView topLeftCell="F1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="V19" sqref="V19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.28515625" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="11.42578125" style="1"/>
+    <col min="1" max="1" width="4.25" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="11.375" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" s="8" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -7321,26 +7349,26 @@
       <selection pane="bottomLeft" activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="1.5703125" style="30" customWidth="1"/>
+    <col min="1" max="1" width="1.625" style="30" customWidth="1"/>
     <col min="2" max="2" width="25" style="10" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" style="10" customWidth="1"/>
-    <col min="4" max="4" width="8.42578125" style="10" customWidth="1"/>
-    <col min="5" max="5" width="41.85546875" style="10" customWidth="1"/>
-    <col min="6" max="6" width="103.42578125" style="10" customWidth="1"/>
-    <col min="7" max="16384" width="11.42578125" style="10"/>
+    <col min="3" max="3" width="15.75" style="10" customWidth="1"/>
+    <col min="4" max="4" width="8.375" style="10" customWidth="1"/>
+    <col min="5" max="5" width="41.875" style="10" customWidth="1"/>
+    <col min="6" max="6" width="103.375" style="10" customWidth="1"/>
+    <col min="7" max="16384" width="11.375" style="10"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="24" customFormat="1" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="25"/>
-      <c r="B1" s="48" t="s">
+      <c r="B1" s="51" t="s">
         <v>219</v>
       </c>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
-      <c r="F1" s="48"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
+      <c r="F1" s="51"/>
     </row>
     <row r="2" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="26"/>
@@ -7703,27 +7731,27 @@
       <selection pane="bottomLeft" activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="1.5703125" style="30" customWidth="1"/>
+    <col min="1" max="1" width="1.625" style="30" customWidth="1"/>
     <col min="2" max="2" width="25" style="10" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" style="10" customWidth="1"/>
-    <col min="4" max="4" width="8.42578125" style="10" customWidth="1"/>
-    <col min="5" max="5" width="43.85546875" style="10" customWidth="1"/>
-    <col min="6" max="6" width="103.42578125" style="10" customWidth="1"/>
-    <col min="7" max="7" width="19.42578125" style="10" customWidth="1"/>
-    <col min="8" max="16384" width="11.42578125" style="10"/>
+    <col min="3" max="3" width="15.75" style="10" customWidth="1"/>
+    <col min="4" max="4" width="8.375" style="10" customWidth="1"/>
+    <col min="5" max="5" width="43.875" style="10" customWidth="1"/>
+    <col min="6" max="6" width="103.375" style="10" customWidth="1"/>
+    <col min="7" max="7" width="19.375" style="10" customWidth="1"/>
+    <col min="8" max="16384" width="11.375" style="10"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="24" customFormat="1" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="25"/>
-      <c r="B1" s="48" t="s">
+      <c r="B1" s="51" t="s">
         <v>327</v>
       </c>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
-      <c r="F1" s="48"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
+      <c r="F1" s="51"/>
     </row>
     <row r="2" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="26"/>
@@ -8136,27 +8164,27 @@
       <selection pane="bottomLeft" activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="1.5703125" style="30" customWidth="1"/>
+    <col min="1" max="1" width="1.625" style="30" customWidth="1"/>
     <col min="2" max="2" width="25" style="10" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" style="10" customWidth="1"/>
-    <col min="4" max="4" width="8.42578125" style="10" customWidth="1"/>
-    <col min="5" max="5" width="43.85546875" style="10" customWidth="1"/>
-    <col min="6" max="6" width="103.42578125" style="10" customWidth="1"/>
-    <col min="7" max="7" width="19.42578125" style="10" customWidth="1"/>
-    <col min="8" max="16384" width="11.42578125" style="10"/>
+    <col min="3" max="3" width="15.75" style="10" customWidth="1"/>
+    <col min="4" max="4" width="8.375" style="10" customWidth="1"/>
+    <col min="5" max="5" width="43.875" style="10" customWidth="1"/>
+    <col min="6" max="6" width="103.375" style="10" customWidth="1"/>
+    <col min="7" max="7" width="19.375" style="10" customWidth="1"/>
+    <col min="8" max="16384" width="11.375" style="10"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="24" customFormat="1" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="25"/>
-      <c r="B1" s="48" t="s">
+      <c r="B1" s="51" t="s">
         <v>329</v>
       </c>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
-      <c r="F1" s="48"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
+      <c r="F1" s="51"/>
     </row>
     <row r="2" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="26"/>
@@ -8247,27 +8275,27 @@
       <selection pane="bottomLeft" activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="1.5703125" style="30" customWidth="1"/>
+    <col min="1" max="1" width="1.625" style="30" customWidth="1"/>
     <col min="2" max="2" width="25" style="10" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" style="10" customWidth="1"/>
-    <col min="4" max="4" width="8.42578125" style="10" customWidth="1"/>
-    <col min="5" max="5" width="41.85546875" style="10" customWidth="1"/>
-    <col min="6" max="6" width="40.7109375" style="10" customWidth="1"/>
-    <col min="7" max="7" width="41.5703125" style="10" customWidth="1"/>
-    <col min="8" max="16384" width="11.42578125" style="10"/>
+    <col min="3" max="3" width="15.75" style="10" customWidth="1"/>
+    <col min="4" max="4" width="8.375" style="10" customWidth="1"/>
+    <col min="5" max="5" width="41.875" style="10" customWidth="1"/>
+    <col min="6" max="6" width="40.75" style="10" customWidth="1"/>
+    <col min="7" max="7" width="41.625" style="10" customWidth="1"/>
+    <col min="8" max="16384" width="11.375" style="10"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="24" customFormat="1" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="25"/>
-      <c r="B1" s="49" t="s">
+      <c r="B1" s="52" t="s">
         <v>334</v>
       </c>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
-      <c r="F1" s="49"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
+      <c r="F1" s="52"/>
     </row>
     <row r="2" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="26"/>
@@ -8327,110 +8355,110 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B6" s="50" t="s">
+      <c r="B6" s="53" t="s">
         <v>263</v>
       </c>
-      <c r="C6" s="50"/>
-      <c r="D6" s="50"/>
-      <c r="E6" s="50"/>
-      <c r="F6" s="50"/>
-      <c r="G6" s="50"/>
+      <c r="C6" s="53"/>
+      <c r="D6" s="53"/>
+      <c r="E6" s="53"/>
+      <c r="F6" s="53"/>
+      <c r="G6" s="53"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B7" s="50"/>
-      <c r="C7" s="50"/>
-      <c r="D7" s="50"/>
-      <c r="E7" s="50"/>
-      <c r="F7" s="50"/>
-      <c r="G7" s="50"/>
+      <c r="B7" s="53"/>
+      <c r="C7" s="53"/>
+      <c r="D7" s="53"/>
+      <c r="E7" s="53"/>
+      <c r="F7" s="53"/>
+      <c r="G7" s="53"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B8" s="50"/>
-      <c r="C8" s="50"/>
-      <c r="D8" s="50"/>
-      <c r="E8" s="50"/>
-      <c r="F8" s="50"/>
-      <c r="G8" s="50"/>
+      <c r="B8" s="53"/>
+      <c r="C8" s="53"/>
+      <c r="D8" s="53"/>
+      <c r="E8" s="53"/>
+      <c r="F8" s="53"/>
+      <c r="G8" s="53"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B9" s="50"/>
-      <c r="C9" s="50"/>
-      <c r="D9" s="50"/>
-      <c r="E9" s="50"/>
-      <c r="F9" s="50"/>
-      <c r="G9" s="50"/>
+      <c r="B9" s="53"/>
+      <c r="C9" s="53"/>
+      <c r="D9" s="53"/>
+      <c r="E9" s="53"/>
+      <c r="F9" s="53"/>
+      <c r="G9" s="53"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B10" s="50"/>
-      <c r="C10" s="50"/>
-      <c r="D10" s="50"/>
-      <c r="E10" s="50"/>
-      <c r="F10" s="50"/>
-      <c r="G10" s="50"/>
+      <c r="B10" s="53"/>
+      <c r="C10" s="53"/>
+      <c r="D10" s="53"/>
+      <c r="E10" s="53"/>
+      <c r="F10" s="53"/>
+      <c r="G10" s="53"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B11" s="50"/>
-      <c r="C11" s="50"/>
-      <c r="D11" s="50"/>
-      <c r="E11" s="50"/>
-      <c r="F11" s="50"/>
-      <c r="G11" s="50"/>
+      <c r="B11" s="53"/>
+      <c r="C11" s="53"/>
+      <c r="D11" s="53"/>
+      <c r="E11" s="53"/>
+      <c r="F11" s="53"/>
+      <c r="G11" s="53"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B12" s="50"/>
-      <c r="C12" s="50"/>
-      <c r="D12" s="50"/>
-      <c r="E12" s="50"/>
-      <c r="F12" s="50"/>
-      <c r="G12" s="50"/>
+      <c r="B12" s="53"/>
+      <c r="C12" s="53"/>
+      <c r="D12" s="53"/>
+      <c r="E12" s="53"/>
+      <c r="F12" s="53"/>
+      <c r="G12" s="53"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B13" s="50"/>
-      <c r="C13" s="50"/>
-      <c r="D13" s="50"/>
-      <c r="E13" s="50"/>
-      <c r="F13" s="50"/>
-      <c r="G13" s="50"/>
+      <c r="B13" s="53"/>
+      <c r="C13" s="53"/>
+      <c r="D13" s="53"/>
+      <c r="E13" s="53"/>
+      <c r="F13" s="53"/>
+      <c r="G13" s="53"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B14" s="50"/>
-      <c r="C14" s="50"/>
-      <c r="D14" s="50"/>
-      <c r="E14" s="50"/>
-      <c r="F14" s="50"/>
-      <c r="G14" s="50"/>
+      <c r="B14" s="53"/>
+      <c r="C14" s="53"/>
+      <c r="D14" s="53"/>
+      <c r="E14" s="53"/>
+      <c r="F14" s="53"/>
+      <c r="G14" s="53"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B15" s="50"/>
-      <c r="C15" s="50"/>
-      <c r="D15" s="50"/>
-      <c r="E15" s="50"/>
-      <c r="F15" s="50"/>
-      <c r="G15" s="50"/>
+      <c r="B15" s="53"/>
+      <c r="C15" s="53"/>
+      <c r="D15" s="53"/>
+      <c r="E15" s="53"/>
+      <c r="F15" s="53"/>
+      <c r="G15" s="53"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B16" s="50"/>
-      <c r="C16" s="50"/>
-      <c r="D16" s="50"/>
-      <c r="E16" s="50"/>
-      <c r="F16" s="50"/>
-      <c r="G16" s="50"/>
+      <c r="B16" s="53"/>
+      <c r="C16" s="53"/>
+      <c r="D16" s="53"/>
+      <c r="E16" s="53"/>
+      <c r="F16" s="53"/>
+      <c r="G16" s="53"/>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B17" s="50"/>
-      <c r="C17" s="50"/>
-      <c r="D17" s="50"/>
-      <c r="E17" s="50"/>
-      <c r="F17" s="50"/>
-      <c r="G17" s="50"/>
+      <c r="B17" s="53"/>
+      <c r="C17" s="53"/>
+      <c r="D17" s="53"/>
+      <c r="E17" s="53"/>
+      <c r="F17" s="53"/>
+      <c r="G17" s="53"/>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B18" s="50"/>
-      <c r="C18" s="50"/>
-      <c r="D18" s="50"/>
-      <c r="E18" s="50"/>
-      <c r="F18" s="50"/>
-      <c r="G18" s="50"/>
+      <c r="B18" s="53"/>
+      <c r="C18" s="53"/>
+      <c r="D18" s="53"/>
+      <c r="E18" s="53"/>
+      <c r="F18" s="53"/>
+      <c r="G18" s="53"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -8454,27 +8482,27 @@
       <selection pane="bottomLeft" activeCell="A9" sqref="A9:XFD9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="1.5703125" style="30" customWidth="1"/>
+    <col min="1" max="1" width="1.625" style="30" customWidth="1"/>
     <col min="2" max="2" width="25" style="10" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" style="10" customWidth="1"/>
-    <col min="4" max="4" width="8.42578125" style="10" customWidth="1"/>
-    <col min="5" max="5" width="41.85546875" style="10" customWidth="1"/>
-    <col min="6" max="6" width="40.7109375" style="10" customWidth="1"/>
-    <col min="7" max="7" width="17.7109375" style="10" customWidth="1"/>
-    <col min="8" max="16384" width="11.42578125" style="10"/>
+    <col min="3" max="3" width="15.75" style="10" customWidth="1"/>
+    <col min="4" max="4" width="8.375" style="10" customWidth="1"/>
+    <col min="5" max="5" width="41.875" style="10" customWidth="1"/>
+    <col min="6" max="6" width="40.75" style="10" customWidth="1"/>
+    <col min="7" max="7" width="17.75" style="10" customWidth="1"/>
+    <col min="8" max="16384" width="11.375" style="10"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="24" customFormat="1" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="25"/>
-      <c r="B1" s="48" t="s">
+      <c r="B1" s="51" t="s">
         <v>224</v>
       </c>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
-      <c r="F1" s="48"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
+      <c r="F1" s="51"/>
     </row>
     <row r="2" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="26"/>
@@ -8624,27 +8652,27 @@
       <selection pane="bottomLeft" activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="1.5703125" style="30" customWidth="1"/>
+    <col min="1" max="1" width="1.625" style="30" customWidth="1"/>
     <col min="2" max="2" width="25" style="10" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" style="10" customWidth="1"/>
-    <col min="4" max="4" width="8.42578125" style="10" customWidth="1"/>
-    <col min="5" max="5" width="41.85546875" style="10" customWidth="1"/>
+    <col min="3" max="3" width="15.75" style="10" customWidth="1"/>
+    <col min="4" max="4" width="8.375" style="10" customWidth="1"/>
+    <col min="5" max="5" width="41.875" style="10" customWidth="1"/>
     <col min="6" max="6" width="43" style="10" customWidth="1"/>
-    <col min="7" max="7" width="17.5703125" style="10" customWidth="1"/>
-    <col min="8" max="16384" width="11.42578125" style="10"/>
+    <col min="7" max="7" width="17.625" style="10" customWidth="1"/>
+    <col min="8" max="16384" width="11.375" style="10"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="24" customFormat="1" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="25"/>
-      <c r="B1" s="48" t="s">
+      <c r="B1" s="51" t="s">
         <v>225</v>
       </c>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
-      <c r="F1" s="48"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
+      <c r="F1" s="51"/>
     </row>
     <row r="2" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="26"/>
@@ -8769,27 +8797,27 @@
       <selection pane="bottomLeft" activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="1.5703125" style="30" customWidth="1"/>
+    <col min="1" max="1" width="1.625" style="30" customWidth="1"/>
     <col min="2" max="2" width="25" style="10" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" style="10" customWidth="1"/>
-    <col min="4" max="4" width="8.42578125" style="10" customWidth="1"/>
-    <col min="5" max="5" width="41.85546875" style="10" customWidth="1"/>
-    <col min="6" max="6" width="72.42578125" style="10" customWidth="1"/>
+    <col min="3" max="3" width="15.75" style="10" customWidth="1"/>
+    <col min="4" max="4" width="8.375" style="10" customWidth="1"/>
+    <col min="5" max="5" width="41.875" style="10" customWidth="1"/>
+    <col min="6" max="6" width="72.375" style="10" customWidth="1"/>
     <col min="7" max="7" width="30" style="10" customWidth="1"/>
-    <col min="8" max="16384" width="11.42578125" style="10"/>
+    <col min="8" max="16384" width="11.375" style="10"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="24" customFormat="1" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="25"/>
-      <c r="B1" s="48" t="s">
+      <c r="B1" s="51" t="s">
         <v>231</v>
       </c>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
-      <c r="F1" s="48"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
+      <c r="F1" s="51"/>
     </row>
     <row r="2" spans="1:7" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="26"/>

</xml_diff>